<commit_message>
cleaned up tables and supplemental tables
</commit_message>
<xml_diff>
--- a/Tables/ppm_AsSugPeLs.xlsx
+++ b/Tables/ppm_AsSugPeLs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineheal/Google_Drive/Shared drives/KHeal_backupfiles/0_Manuscripts/_Heal_ParticulateArsenicPools/ParticulateAs_DataProcessing/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F193C3D4-26AE-1C4F-A294-4780C2873D70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD9C61C-635F-8943-B8A6-67FC815C6D1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2860" yWindow="3160" windowWidth="19500" windowHeight="17440" xr2:uid="{F8372F0B-1424-2B46-BE3E-1844004A2124}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F10" sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>